<commit_message>
update for crypto futures and perpetuals
</commit_message>
<xml_diff>
--- a/examples/crypto/positions.xlsx
+++ b/examples/crypto/positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bilal/Documents/git/portfolio-stress-test/examples/crypto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81589C4-C207-CE42-82D4-9C109A45AB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB8E607-2B6C-7449-9284-9F1AD89F72E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="680" windowWidth="25440" windowHeight="14340" xr2:uid="{20790C52-6D9F-4F48-87DC-BDC9F65E5FFA}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{20790C52-6D9F-4F48-87DC-BDC9F65E5FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>instrument</t>
   </si>
@@ -44,88 +44,25 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>BTC-25OCT24-50000-P</t>
-  </si>
-  <si>
-    <t>BTC-25OCT24-84000-C</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-43000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-44000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-45000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-47000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-48000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-49000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-52000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-53000-P</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-90000-C</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-47000-P</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-48000-P</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-49000-P</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-50000-P</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-80000-C</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-85000-C</t>
-  </si>
-  <si>
-    <t>BTC-27SEP24-90000-C</t>
-  </si>
-  <si>
-    <t>BTC-30AUG24-75000-C</t>
-  </si>
-  <si>
-    <t>BTC-30AUG24-82000-C</t>
-  </si>
-  <si>
     <t>BTC-27DEC24-105000-C</t>
   </si>
   <si>
-    <t>BTC-27DEC24-110000-C</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-115000-C</t>
-  </si>
-  <si>
-    <t>BTC-27DEC24-120000-C</t>
-  </si>
-  <si>
-    <t>BTC-28MAR25-120000-C</t>
-  </si>
-  <si>
-    <t>BTC-28MAR25-130000-C</t>
-  </si>
-  <si>
-    <t>BTC-28MAR25-140000-C</t>
-  </si>
-  <si>
-    <t>BTC-28MAR25-150000-C</t>
+    <t>BTC-27DEC24</t>
+  </si>
+  <si>
+    <t>BTC-PERPETUAL</t>
+  </si>
+  <si>
+    <t>BTC-25OCT24-44000-P</t>
+  </si>
+  <si>
+    <t>BTC-25OCT24-45000-P</t>
+  </si>
+  <si>
+    <t>BTC-27DEC24-100000-C</t>
+  </si>
+  <si>
+    <t>BTC</t>
   </si>
 </sst>
 </file>
@@ -515,7 +452,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,10 +470,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>-25</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -544,216 +481,121 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>-8.8000000000000007</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>-28.9</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>-1.7</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>95</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>31.4</v>
+        <v>-230</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
-        <v>20.6</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>14</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-9</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2">
-        <v>-9.1999999999999993</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-25</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2">
-        <v>-18.7</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2">
-        <v>-4.2</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2">
-        <v>18.600000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2">
-        <v>79.599999999999994</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2">
-        <v>37.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="2">
-        <v>201.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="2">
-        <v>72.400000000000006</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2">
-        <v>-209.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2">
-        <v>-154.30000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="2">
-        <v>-105.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="2">
-        <v>-67.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="2">
-        <v>12</v>
-      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>